<commit_message>
additions to select school data file
</commit_message>
<xml_diff>
--- a/data/select_school_surveys.xlsx
+++ b/data/select_school_surveys.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.alvarez/Documents/tutorials_and_examples/school-quality-dashboard/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7625C1-FEC5-C446-B094-0A207028B15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25360" windowHeight="16320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>school</t>
   </si>
@@ -130,12 +136,30 @@
   </si>
   <si>
     <t>forest-hills</t>
+  </si>
+  <si>
+    <t>teachers_recommend_school_to_families</t>
+  </si>
+  <si>
+    <t>q151</t>
+  </si>
+  <si>
+    <t>q148</t>
+  </si>
+  <si>
+    <t>q361</t>
+  </si>
+  <si>
+    <t>woodside</t>
+  </si>
+  <si>
+    <t>east-elmhurst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -179,6 +203,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -503,14 +535,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,8 +623,11 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -669,8 +706,11 @@
       <c r="Z2" s="1">
         <v>97</v>
       </c>
+      <c r="AA2" s="1">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -749,8 +789,11 @@
       <c r="Z3" s="1">
         <v>96</v>
       </c>
+      <c r="AA3" s="1">
+        <v>95</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -829,8 +872,11 @@
       <c r="Z4" s="1">
         <v>96</v>
       </c>
+      <c r="AA4" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -909,8 +955,11 @@
       <c r="Z5" s="1">
         <v>96</v>
       </c>
+      <c r="AA5" s="1">
+        <v>83</v>
+      </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -989,8 +1038,11 @@
       <c r="Z6" s="1">
         <v>98</v>
       </c>
+      <c r="AA6" s="1">
+        <v>89</v>
+      </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1067,8 +1119,11 @@
       <c r="Z7" s="1">
         <v>96</v>
       </c>
+      <c r="AA7" s="1">
+        <v>89</v>
+      </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1147,8 +1202,11 @@
       <c r="Z8" s="1">
         <v>94</v>
       </c>
+      <c r="AA8" s="1">
+        <v>98</v>
+      </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1226,6 +1284,258 @@
       </c>
       <c r="Z9" s="1">
         <v>94</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>68</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>84</v>
+      </c>
+      <c r="G10" s="1">
+        <v>89</v>
+      </c>
+      <c r="H10" s="1">
+        <v>99</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+      <c r="J10" s="1">
+        <v>97</v>
+      </c>
+      <c r="K10" s="1">
+        <v>100</v>
+      </c>
+      <c r="L10" s="1">
+        <v>98</v>
+      </c>
+      <c r="M10" s="1">
+        <v>99</v>
+      </c>
+      <c r="N10" s="1">
+        <v>97</v>
+      </c>
+      <c r="O10" s="1">
+        <v>98</v>
+      </c>
+      <c r="P10" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>99</v>
+      </c>
+      <c r="R10" s="1">
+        <v>97</v>
+      </c>
+      <c r="S10" s="1">
+        <v>95</v>
+      </c>
+      <c r="T10" s="1">
+        <v>97</v>
+      </c>
+      <c r="U10" s="1">
+        <v>98</v>
+      </c>
+      <c r="V10" s="1">
+        <v>100</v>
+      </c>
+      <c r="W10" s="1">
+        <v>93</v>
+      </c>
+      <c r="X10" s="1">
+        <v>89</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>98</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>100</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1">
+        <v>76</v>
+      </c>
+      <c r="G11" s="1">
+        <v>73</v>
+      </c>
+      <c r="H11" s="1">
+        <v>91</v>
+      </c>
+      <c r="I11" s="1">
+        <v>91</v>
+      </c>
+      <c r="J11" s="1">
+        <v>74</v>
+      </c>
+      <c r="K11" s="1">
+        <v>84</v>
+      </c>
+      <c r="L11" s="1">
+        <v>89</v>
+      </c>
+      <c r="M11" s="1">
+        <v>86</v>
+      </c>
+      <c r="N11" s="1">
+        <v>96</v>
+      </c>
+      <c r="O11" s="1">
+        <v>97</v>
+      </c>
+      <c r="P11" s="1">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>87</v>
+      </c>
+      <c r="R11" s="1">
+        <v>92</v>
+      </c>
+      <c r="S11" s="1">
+        <v>92</v>
+      </c>
+      <c r="T11" s="1">
+        <v>97</v>
+      </c>
+      <c r="U11" s="1">
+        <v>90</v>
+      </c>
+      <c r="V11" s="1">
+        <v>75</v>
+      </c>
+      <c r="W11" s="1">
+        <v>81</v>
+      </c>
+      <c r="X11" s="1">
+        <v>87</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>88</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>98</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1">
+        <v>81</v>
+      </c>
+      <c r="F12" s="1">
+        <v>84</v>
+      </c>
+      <c r="G12" s="1">
+        <v>83</v>
+      </c>
+      <c r="H12" s="1">
+        <v>99</v>
+      </c>
+      <c r="I12" s="1">
+        <v>97</v>
+      </c>
+      <c r="J12" s="1">
+        <v>99</v>
+      </c>
+      <c r="K12" s="1">
+        <v>98</v>
+      </c>
+      <c r="L12" s="1">
+        <v>89</v>
+      </c>
+      <c r="M12" s="1">
+        <v>95</v>
+      </c>
+      <c r="N12" s="1">
+        <v>98</v>
+      </c>
+      <c r="O12" s="1">
+        <v>98</v>
+      </c>
+      <c r="P12" s="1">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>99</v>
+      </c>
+      <c r="R12" s="1">
+        <v>98</v>
+      </c>
+      <c r="S12" s="1">
+        <v>96</v>
+      </c>
+      <c r="T12" s="1">
+        <v>96</v>
+      </c>
+      <c r="U12" s="1">
+        <v>94</v>
+      </c>
+      <c r="V12" s="1">
+        <v>94</v>
+      </c>
+      <c r="W12" s="1">
+        <v>85</v>
+      </c>
+      <c r="X12" s="1">
+        <v>87</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>98</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>100</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>